<commit_message>
vco: intro, vco, tl
</commit_message>
<xml_diff>
--- a/Ej3/Mediciones/tc_tp6_ej3_jitter.xlsx
+++ b/Ej3/Mediciones/tc_tp6_ej3_jitter.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rochi\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rochi\Google Drive\Materias\Teoría de circuitos\TPs\TC_TP6\Ej3\Mediciones\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A2" sqref="A2:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,125 +424,128 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>10.07</v>
+        <v>1.123</v>
       </c>
       <c r="C2">
-        <v>10</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="D2">
-        <v>10.199999999999999</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="E2" s="1">
-        <v>4.3999999999999997E-2</v>
+        <v>2.0999999999999999E-3</v>
       </c>
       <c r="F2">
-        <v>1.99</v>
+        <v>1.96</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4.0999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="B3">
-        <v>8.49</v>
+        <v>3.22</v>
       </c>
       <c r="C3">
-        <v>8.4</v>
+        <v>3.21</v>
       </c>
       <c r="D3">
-        <v>8.6</v>
+        <v>3.23</v>
       </c>
       <c r="E3" s="1">
-        <v>2.4E-2</v>
+        <v>6.6E-3</v>
       </c>
       <c r="F3">
-        <v>1.99</v>
+        <v>1.97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>6.76</v>
+        <v>4.88</v>
       </c>
       <c r="C4">
-        <v>6.71</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D4">
-        <v>6.8</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E4" s="1">
-        <v>1.4999999999999999E-2</v>
+        <v>4.7000000000000002E-3</v>
       </c>
       <c r="F4">
-        <v>1.99</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>3.1</v>
       </c>
       <c r="B5">
-        <v>4.88</v>
+        <v>6.76</v>
       </c>
       <c r="C5">
-        <v>4.8499999999999996</v>
+        <v>6.71</v>
       </c>
       <c r="D5">
-        <v>4.9000000000000004</v>
+        <v>6.8</v>
       </c>
       <c r="E5" s="1">
-        <v>4.7000000000000002E-3</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="F5">
-        <v>1.98</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>1.1000000000000001</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="B6">
-        <v>3.22</v>
+        <v>8.49</v>
       </c>
       <c r="C6">
-        <v>3.21</v>
+        <v>8.4</v>
       </c>
       <c r="D6">
-        <v>3.23</v>
+        <v>8.6</v>
       </c>
       <c r="E6" s="1">
-        <v>6.6E-3</v>
+        <v>2.4E-2</v>
       </c>
       <c r="F6">
-        <v>1.97</v>
+        <v>1.99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>1.123</v>
+        <v>10.07</v>
       </c>
       <c r="C7">
-        <v>1.1200000000000001</v>
+        <v>10</v>
       </c>
       <c r="D7">
-        <v>1.1299999999999999</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E7" s="1">
-        <v>2.0999999999999999E-3</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="F7">
-        <v>1.96</v>
+        <v>1.99</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F7">
+    <sortCondition ref="A2:A7"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>